<commit_message>
send final versions of DDE related files to github
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -139,16 +139,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -164,12 +164,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="156295168"/>
-        <c:axId val="156296704"/>
+        <c:axId val="153160704"/>
+        <c:axId val="153187072"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="156295168"/>
+        <c:axId val="153160704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -178,7 +178,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156296704"/>
+        <c:crossAx val="153187072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -186,7 +186,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="156296704"/>
+        <c:axId val="153187072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -197,7 +197,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156295168"/>
+        <c:crossAx val="153160704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -223,16 +223,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>80962</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>606592</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>100264</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>385762</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>390774</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>66926</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -258,13 +258,6 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <ddeLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ddeService="prolog" ddeTopic="current_prolog_flag">
     <ddeItems>
-      <ddeItem name="home" advise="1">
-        <values>
-          <value t="str">
-            <val>c:/program files/swipl</val>
-          </value>
-        </values>
-      </ddeItem>
       <ddeItem name="StdDocumentName" ole="1" advise="1"/>
       <ddeItem name="version" advise="1">
         <values>
@@ -567,9 +560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -592,24 +583,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="L1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M1">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -854,9 +845,9 @@
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" t="str">
-        <f>[1]!home</f>
-        <v>c:/program files/swipl</v>
+      <c r="F17">
+        <f>[1]!version</f>
+        <v>70321</v>
       </c>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>